<commit_message>
plot all the time series plots (both mean and median) moments by different group.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/micro_reg.xlsx
+++ b/WorkingFolder/Tables/micro_reg.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>incvar I</t>
   </si>
@@ -61,6 +61,9 @@
     <t>Stkprob</t>
   </si>
   <si>
+    <t>UEprobAgg</t>
+  </si>
+  <si>
     <t>UEprobInd</t>
   </si>
   <si>
@@ -70,166 +73,172 @@
     <t>R2</t>
   </si>
   <si>
+    <t>0.25*</t>
+  </si>
+  <si>
+    <t>(0.13)</t>
+  </si>
+  <si>
+    <t>7.58***</t>
+  </si>
+  <si>
+    <t>(0.15)</t>
+  </si>
+  <si>
+    <t>4.62***</t>
+  </si>
+  <si>
+    <t>(0.05)</t>
+  </si>
+  <si>
     <t>0.05</t>
   </si>
   <si>
+    <t>51788</t>
+  </si>
+  <si>
+    <t>0.35***</t>
+  </si>
+  <si>
+    <t>-0.00</t>
+  </si>
+  <si>
+    <t>(0.00)</t>
+  </si>
+  <si>
+    <t>3.76***</t>
+  </si>
+  <si>
     <t>(0.12)</t>
   </si>
   <si>
-    <t>7.21***</t>
-  </si>
-  <si>
-    <t>(0.15)</t>
-  </si>
-  <si>
-    <t>4.64***</t>
-  </si>
-  <si>
-    <t>(0.05)</t>
-  </si>
-  <si>
-    <t>54029</t>
-  </si>
-  <si>
-    <t>0.24*</t>
-  </si>
-  <si>
-    <t>(0.13)</t>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>0.01***</t>
+  </si>
+  <si>
+    <t>0.00**</t>
+  </si>
+  <si>
+    <t>0.03***</t>
+  </si>
+  <si>
+    <t>45903</t>
+  </si>
+  <si>
+    <t>1.52***</t>
+  </si>
+  <si>
+    <t>(0.10)</t>
+  </si>
+  <si>
+    <t>-0.02</t>
+  </si>
+  <si>
+    <t>(0.14)</t>
+  </si>
+  <si>
+    <t>-0.00**</t>
+  </si>
+  <si>
+    <t>3.30***</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.44***</t>
+  </si>
+  <si>
+    <t>-0.82***</t>
+  </si>
+  <si>
+    <t>5.71***</t>
+  </si>
+  <si>
+    <t>(0.08)</t>
+  </si>
+  <si>
+    <t>45430</t>
+  </si>
+  <si>
+    <t>1.90***</t>
+  </si>
+  <si>
+    <t>(0.25)</t>
+  </si>
+  <si>
+    <t>6.72***</t>
+  </si>
+  <si>
+    <t>(0.29)</t>
+  </si>
+  <si>
+    <t>12.42***</t>
+  </si>
+  <si>
+    <t>48665</t>
+  </si>
+  <si>
+    <t>2.23***</t>
+  </si>
+  <si>
+    <t>(0.27)</t>
   </si>
   <si>
     <t>-0.00***</t>
   </si>
   <si>
-    <t>(0.00)</t>
-  </si>
-  <si>
-    <t>3.91***</t>
-  </si>
-  <si>
-    <t>(0.10)</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>0.01***</t>
-  </si>
-  <si>
-    <t>0.03***</t>
-  </si>
-  <si>
-    <t>47356</t>
-  </si>
-  <si>
-    <t>1.57***</t>
-  </si>
-  <si>
-    <t>-0.12</t>
-  </si>
-  <si>
-    <t>3.39***</t>
-  </si>
-  <si>
-    <t>(0.11)</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>0.40***</t>
-  </si>
-  <si>
-    <t>-0.80***</t>
-  </si>
-  <si>
-    <t>5.72***</t>
-  </si>
-  <si>
-    <t>(0.07)</t>
-  </si>
-  <si>
-    <t>47457</t>
-  </si>
-  <si>
-    <t>1.41***</t>
-  </si>
-  <si>
-    <t>(0.23)</t>
-  </si>
-  <si>
-    <t>6.27***</t>
-  </si>
-  <si>
-    <t>(0.27)</t>
-  </si>
-  <si>
-    <t>12.42***</t>
-  </si>
-  <si>
-    <t>50730</t>
-  </si>
-  <si>
-    <t>1.80***</t>
-  </si>
-  <si>
-    <t>(0.26)</t>
-  </si>
-  <si>
-    <t>0.00***</t>
-  </si>
-  <si>
-    <t>13.64***</t>
-  </si>
-  <si>
-    <t>(0.21)</t>
+    <t>12.26***</t>
+  </si>
+  <si>
+    <t>-0.06***</t>
+  </si>
+  <si>
+    <t>0.05***</t>
+  </si>
+  <si>
+    <t>43077</t>
+  </si>
+  <si>
+    <t>6.97***</t>
+  </si>
+  <si>
+    <t>(0.20)</t>
+  </si>
+  <si>
+    <t>0.56**</t>
+  </si>
+  <si>
+    <t>10.22***</t>
+  </si>
+  <si>
+    <t>0.04</t>
   </si>
   <si>
     <t>-0.05***</t>
   </si>
   <si>
-    <t>0.06***</t>
-  </si>
-  <si>
-    <t>44404</t>
-  </si>
-  <si>
-    <t>7.09***</t>
+    <t>0.04***</t>
+  </si>
+  <si>
+    <t>4.01***</t>
+  </si>
+  <si>
+    <t>(0.22)</t>
+  </si>
+  <si>
+    <t>2.67***</t>
   </si>
   <si>
     <t>(0.19)</t>
   </si>
   <si>
-    <t>0.16</t>
-  </si>
-  <si>
-    <t>11.36***</t>
-  </si>
-  <si>
-    <t>(0.22)</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>-0.04***</t>
-  </si>
-  <si>
-    <t>0.05***</t>
-  </si>
-  <si>
-    <t>3.82***</t>
-  </si>
-  <si>
-    <t>2.76***</t>
-  </si>
-  <si>
-    <t>11.16***</t>
-  </si>
-  <si>
-    <t>(0.14)</t>
-  </si>
-  <si>
-    <t>44517</t>
+    <t>11.21***</t>
+  </si>
+  <si>
+    <t>42654</t>
   </si>
 </sst>
 </file>
@@ -587,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,19 +633,19 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -644,19 +653,19 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1"/>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -664,19 +673,19 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -684,43 +693,43 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -728,43 +737,43 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -772,82 +781,82 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -855,31 +864,31 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -887,89 +896,121 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1"/>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="1"/>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" t="s">
-        <v>39</v>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scatter and regression of perceived risk and experienced volatility
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/micro_reg.xlsx
+++ b/WorkingFolder/Tables/micro_reg.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="93">
   <si>
     <t>incvar I</t>
   </si>
@@ -67,6 +67,9 @@
     <t>UEprobInd</t>
   </si>
   <si>
+    <t>rmse</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
@@ -97,145 +100,196 @@
     <t>51788</t>
   </si>
   <si>
-    <t>0.35***</t>
-  </si>
-  <si>
-    <t>-0.00</t>
+    <t>0.30*</t>
+  </si>
+  <si>
+    <t>(0.16)</t>
+  </si>
+  <si>
+    <t>0.00***</t>
   </si>
   <si>
     <t>(0.00)</t>
   </si>
   <si>
-    <t>3.76***</t>
+    <t>-16.31***</t>
+  </si>
+  <si>
+    <t>(2.34)</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.01***</t>
+  </si>
+  <si>
+    <t>0.00*</t>
+  </si>
+  <si>
+    <t>0.02***</t>
+  </si>
+  <si>
+    <t>31.23***</t>
+  </si>
+  <si>
+    <t>(3.63)</t>
+  </si>
+  <si>
+    <t>34391</t>
+  </si>
+  <si>
+    <t>1.45***</t>
+  </si>
+  <si>
+    <t>(0.11)</t>
+  </si>
+  <si>
+    <t>-0.04</t>
+  </si>
+  <si>
+    <t>-0.00***</t>
+  </si>
+  <si>
+    <t>-17.19***</t>
+  </si>
+  <si>
+    <t>(2.33)</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>31.92***</t>
+  </si>
+  <si>
+    <t>(3.62)</t>
+  </si>
+  <si>
+    <t>0.44***</t>
   </si>
   <si>
     <t>(0.12)</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>0.01***</t>
-  </si>
-  <si>
-    <t>0.00**</t>
+    <t>-0.82***</t>
+  </si>
+  <si>
+    <t>(0.10)</t>
+  </si>
+  <si>
+    <t>5.71***</t>
+  </si>
+  <si>
+    <t>(0.08)</t>
+  </si>
+  <si>
+    <t>45430</t>
+  </si>
+  <si>
+    <t>1.90***</t>
+  </si>
+  <si>
+    <t>(0.25)</t>
+  </si>
+  <si>
+    <t>6.72***</t>
+  </si>
+  <si>
+    <t>(0.29)</t>
+  </si>
+  <si>
+    <t>12.42***</t>
+  </si>
+  <si>
+    <t>48665</t>
+  </si>
+  <si>
+    <t>1.99***</t>
+  </si>
+  <si>
+    <t>(0.31)</t>
+  </si>
+  <si>
+    <t>-11.33**</t>
+  </si>
+  <si>
+    <t>(4.73)</t>
+  </si>
+  <si>
+    <t>-0.06***</t>
+  </si>
+  <si>
+    <t>0.06***</t>
+  </si>
+  <si>
+    <t>0.04***</t>
+  </si>
+  <si>
+    <t>(0.01)</t>
+  </si>
+  <si>
+    <t>36.59***</t>
+  </si>
+  <si>
+    <t>(7.33)</t>
+  </si>
+  <si>
+    <t>32323</t>
+  </si>
+  <si>
+    <t>6.66***</t>
+  </si>
+  <si>
+    <t>(0.23)</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>(0.32)</t>
+  </si>
+  <si>
+    <t>-15.35***</t>
+  </si>
+  <si>
+    <t>(4.67)</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>-0.05***</t>
+  </si>
+  <si>
+    <t>0.05***</t>
   </si>
   <si>
     <t>0.03***</t>
   </si>
   <si>
-    <t>45903</t>
-  </si>
-  <si>
-    <t>1.52***</t>
-  </si>
-  <si>
-    <t>(0.10)</t>
-  </si>
-  <si>
-    <t>-0.02</t>
+    <t>39.80***</t>
+  </si>
+  <si>
+    <t>(7.24)</t>
+  </si>
+  <si>
+    <t>4.01***</t>
+  </si>
+  <si>
+    <t>(0.22)</t>
+  </si>
+  <si>
+    <t>2.67***</t>
+  </si>
+  <si>
+    <t>(0.19)</t>
+  </si>
+  <si>
+    <t>11.21***</t>
   </si>
   <si>
     <t>(0.14)</t>
-  </si>
-  <si>
-    <t>-0.00**</t>
-  </si>
-  <si>
-    <t>3.30***</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>0.44***</t>
-  </si>
-  <si>
-    <t>-0.82***</t>
-  </si>
-  <si>
-    <t>5.71***</t>
-  </si>
-  <si>
-    <t>(0.08)</t>
-  </si>
-  <si>
-    <t>45430</t>
-  </si>
-  <si>
-    <t>1.90***</t>
-  </si>
-  <si>
-    <t>(0.25)</t>
-  </si>
-  <si>
-    <t>6.72***</t>
-  </si>
-  <si>
-    <t>(0.29)</t>
-  </si>
-  <si>
-    <t>12.42***</t>
-  </si>
-  <si>
-    <t>48665</t>
-  </si>
-  <si>
-    <t>2.23***</t>
-  </si>
-  <si>
-    <t>(0.27)</t>
-  </si>
-  <si>
-    <t>-0.00***</t>
-  </si>
-  <si>
-    <t>12.26***</t>
-  </si>
-  <si>
-    <t>-0.06***</t>
-  </si>
-  <si>
-    <t>0.05***</t>
-  </si>
-  <si>
-    <t>43077</t>
-  </si>
-  <si>
-    <t>6.97***</t>
-  </si>
-  <si>
-    <t>(0.20)</t>
-  </si>
-  <si>
-    <t>0.56**</t>
-  </si>
-  <si>
-    <t>10.22***</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>-0.05***</t>
-  </si>
-  <si>
-    <t>0.04***</t>
-  </si>
-  <si>
-    <t>4.01***</t>
-  </si>
-  <si>
-    <t>(0.22)</t>
-  </si>
-  <si>
-    <t>2.67***</t>
-  </si>
-  <si>
-    <t>(0.19)</t>
-  </si>
-  <si>
-    <t>11.21***</t>
   </si>
   <si>
     <t>42654</t>
@@ -596,7 +650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -633,19 +687,19 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -653,19 +707,19 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1"/>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -673,19 +727,19 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -693,43 +747,43 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -737,43 +791,43 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -781,82 +835,82 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -864,31 +918,31 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -896,31 +950,31 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1"/>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -928,89 +982,121 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1"/>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1"/>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" t="s">
-        <v>43</v>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added numeracy in regression.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/micro_reg.xlsx
+++ b/WorkingFolder/Tables/micro_reg.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>incvar I</t>
   </si>
@@ -55,6 +55,9 @@
     <t>gender=male</t>
   </si>
   <si>
+    <t>nlit_gr=low nlit</t>
+  </si>
+  <si>
     <t>parttime=yes</t>
   </si>
   <si>
@@ -73,115 +76,118 @@
     <t>R2</t>
   </si>
   <si>
-    <t>6.31***</t>
-  </si>
-  <si>
-    <t>(0.40)</t>
-  </si>
-  <si>
-    <t>40529</t>
+    <t>1.19***</t>
+  </si>
+  <si>
+    <t>(0.24)</t>
+  </si>
+  <si>
+    <t>20602</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>1.46***</t>
+  </si>
+  <si>
+    <t>(0.49)</t>
+  </si>
+  <si>
+    <t>-0.12***</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
+  </si>
+  <si>
+    <t>-0.15***</t>
+  </si>
+  <si>
+    <t>-0.16***</t>
+  </si>
+  <si>
+    <t>(0.03)</t>
+  </si>
+  <si>
+    <t>-0.06</t>
+  </si>
+  <si>
+    <t>(0.04)</t>
+  </si>
+  <si>
+    <t>1.53***</t>
+  </si>
+  <si>
+    <t>(0.54)</t>
+  </si>
+  <si>
+    <t>-0.13***</t>
+  </si>
+  <si>
+    <t>-0.17***</t>
+  </si>
+  <si>
+    <t>-0.09**</t>
+  </si>
+  <si>
+    <t>(0.05)</t>
+  </si>
+  <si>
+    <t>0.17***</t>
   </si>
   <si>
     <t>0.01</t>
   </si>
   <si>
-    <t>2.92***</t>
-  </si>
-  <si>
-    <t>(0.83)</t>
-  </si>
-  <si>
-    <t>-0.33***</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
-  </si>
-  <si>
-    <t>-0.51***</t>
-  </si>
-  <si>
-    <t>-0.61***</t>
-  </si>
-  <si>
-    <t>-0.48***</t>
-  </si>
-  <si>
-    <t>(0.04)</t>
+    <t>-0.09***</t>
+  </si>
+  <si>
+    <t>0.06***</t>
+  </si>
+  <si>
+    <t>17456</t>
+  </si>
+  <si>
+    <t>2.47***</t>
+  </si>
+  <si>
+    <t>(0.60)</t>
+  </si>
+  <si>
+    <t>-0.20***</t>
+  </si>
+  <si>
+    <t>-0.21***</t>
+  </si>
+  <si>
+    <t>0.16***</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>-0.06***</t>
+  </si>
+  <si>
+    <t>0.07***</t>
+  </si>
+  <si>
+    <t>-0.00***</t>
+  </si>
+  <si>
+    <t>(0.00)</t>
+  </si>
+  <si>
+    <t>(0.01)</t>
+  </si>
+  <si>
+    <t>0.02***</t>
+  </si>
+  <si>
+    <t>13880</t>
   </si>
   <si>
     <t>0.02</t>
-  </si>
-  <si>
-    <t>3.56***</t>
-  </si>
-  <si>
-    <t>(0.91)</t>
-  </si>
-  <si>
-    <t>-0.34***</t>
-  </si>
-  <si>
-    <t>-0.53***</t>
-  </si>
-  <si>
-    <t>-0.59***</t>
-  </si>
-  <si>
-    <t>(0.05)</t>
-  </si>
-  <si>
-    <t>0.20***</t>
-  </si>
-  <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t>-0.11***</t>
-  </si>
-  <si>
-    <t>-0.38***</t>
-  </si>
-  <si>
-    <t>34101</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>6.15***</t>
-  </si>
-  <si>
-    <t>(0.92)</t>
-  </si>
-  <si>
-    <t>-0.65***</t>
-  </si>
-  <si>
-    <t>-0.58***</t>
-  </si>
-  <si>
-    <t>0.15***</t>
-  </si>
-  <si>
-    <t>-0.08***</t>
-  </si>
-  <si>
-    <t>-0.31***</t>
-  </si>
-  <si>
-    <t>-0.03</t>
-  </si>
-  <si>
-    <t>0.00***</t>
-  </si>
-  <si>
-    <t>(0.00)</t>
-  </si>
-  <si>
-    <t>28898</t>
-  </si>
-  <si>
-    <t>0.05</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,16 +573,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -585,16 +591,16 @@
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>45</v>
@@ -605,31 +611,31 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -637,31 +643,31 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -669,7 +675,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
@@ -678,22 +684,22 @@
         <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -701,31 +707,31 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -733,10 +739,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
         <v>48</v>
@@ -745,13 +751,13 @@
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -771,13 +777,13 @@
     <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -797,27 +803,39 @@
     <row r="17" spans="1:6">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1"/>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -825,13 +843,13 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1"/>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -853,53 +871,67 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
-      </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="1"/>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>43</v>
       </c>
-      <c r="F27" t="s">
-        <v>55</v>
+      <c r="F28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>